<commit_message>
Add Streamlit dashboard for analyzing Taiwan's trade statistics affected by US tariffs
- Created a new Streamlit application (streamlit_analyze.py) to provide an interactive dashboard for analyzing customs import and export trade statistics for Taiwan in 2025.
- Added overall trade data, US trade summary, monthly export and import data, commodity structure, and market export data.
- Implemented various visualizations using Plotly for key metrics, trends, and comparisons.
- Included risk assessment and market analysis sections.
- Added a .gitignore file to exclude virtual environment files.
- Updated requirements.txt with necessary dependencies for the project.
- Added preliminary statistics Excel files for trade data.
</commit_message>
<xml_diff>
--- a/data/August2025_PreliminaryStatistics_on_CustomsImports_and_Exports/Table10_Surplus_inTrade_with_MajorCountries.xlsx
+++ b/data/August2025_PreliminaryStatistics_on_CustomsImports_and_Exports/Table10_Surplus_inTrade_with_MajorCountries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\貿易統計科\記者會資料檔\news上網檔\114年8月\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AboutCoding\CourseCode\Artificial_Intelligence_Practice_CourseCode\ROC_PreliminaryStatistics_on_CustomsImports_and_Exports_for_2025\data\August2025_PreliminaryStatistics_on_CustomsImports_and_Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22F6DF79-3BF0-4A75-BCBB-56829E21862D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6E0994-0881-439C-99D7-05DD94502E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表10" sheetId="1" r:id="rId1"/>
@@ -571,20 +571,6 @@
   </si>
   <si>
     <r>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>月</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>5</t>
     </r>
     <r>
@@ -718,6 +704,21 @@
         <charset val="136"/>
       </rPr>
       <t>」表示入超金額減少。</t>
+    </r>
+    <phoneticPr fontId="25" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>月</t>
     </r>
     <phoneticPr fontId="25" type="noConversion"/>
   </si>
@@ -992,7 +993,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1107,6 +1108,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1608,20 +1621,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
@@ -1645,13 +1655,13 @@
     <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="196" fontId="13" fillId="0" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="196" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="196" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="196" fontId="13" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1670,9 +1680,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1">
@@ -1709,7 +1716,7 @@
     <xf numFmtId="196" fontId="34" fillId="0" borderId="21" xfId="46" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1766,7 +1773,7 @@
     <xf numFmtId="196" fontId="13" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="196" fontId="13" fillId="0" borderId="26" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1775,11 +1782,41 @@
     <xf numFmtId="196" fontId="13" fillId="0" borderId="13" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="196" fontId="13" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="196" fontId="13" fillId="0" borderId="26" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="196" fontId="13" fillId="24" borderId="23" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="196" fontId="13" fillId="24" borderId="24" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="196" fontId="13" fillId="24" borderId="25" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="196" fontId="35" fillId="24" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="34" fillId="24" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="34" fillId="24" borderId="1" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="34" fillId="24" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="196" fontId="34" fillId="24" borderId="21" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="196" fontId="34" fillId="25" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="71">
@@ -1869,12 +1906,9 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="表1"/>
-      <sheetName val="表2"/>
-      <sheetName val="表3"/>
       <sheetName val="表6"/>
       <sheetName val="表7"/>
       <sheetName val="表8"/>
@@ -1886,13 +1920,16 @@
       <sheetName val="匯檔"/>
       <sheetName val="匯率"/>
       <sheetName val="轉檔"/>
-      <sheetName val="國家及洲別代碼"/>
       <sheetName val="進-月"/>
       <sheetName val="參1"/>
       <sheetName val="參2"/>
       <sheetName val="參3"/>
       <sheetName val="參4"/>
       <sheetName val="參5"/>
+      <sheetName val="表1"/>
+      <sheetName val="表2"/>
+      <sheetName val="表3"/>
+      <sheetName val="國家及洲別代碼"/>
       <sheetName val="特國出"/>
       <sheetName val="特國進"/>
       <sheetName val="歐盟出口"/>
@@ -1938,9 +1975,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1978,9 +2015,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2013,26 +2050,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2065,26 +2085,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2261,1486 +2264,1486 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="8" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" sqref="A1:K1"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="23" customWidth="1"/>
-    <col min="2" max="4" width="12.109375" style="28" customWidth="1"/>
-    <col min="5" max="11" width="11.109375" style="28" customWidth="1"/>
-    <col min="12" max="13" width="8.44140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8" style="27"/>
+    <col min="1" max="1" width="16.6640625" style="21" customWidth="1"/>
+    <col min="2" max="4" width="12.109375" style="26" customWidth="1"/>
+    <col min="5" max="11" width="11.109375" style="26" customWidth="1"/>
+    <col min="12" max="13" width="8.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" ht="26.1" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="26.1" customHeight="1">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-    </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-    </row>
-    <row r="3" spans="1:21" s="10" customFormat="1" ht="15.9" customHeight="1" thickBot="1">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+    </row>
+    <row r="2" spans="1:21" s="7" customFormat="1" ht="12" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+    </row>
+    <row r="3" spans="1:21" s="9" customFormat="1" ht="15.9" customHeight="1" thickBot="1">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="17" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:21" s="16" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A4" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="51" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="52" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="17" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="40" t="s">
+    <row r="5" spans="1:21" s="16" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A5" s="45"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="49" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="55"/>
-    </row>
-    <row r="6" spans="1:21" s="17" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="19" t="s">
+      <c r="I5" s="59"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:21" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="46"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="56"/>
-    </row>
-    <row r="7" spans="1:21" s="10" customFormat="1" ht="15.75" hidden="1" customHeight="1">
+      <c r="H6" s="48"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="54"/>
+    </row>
+    <row r="7" spans="1:21" s="9" customFormat="1" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="27">
         <v>48053.495000000003</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="27">
         <v>64877.123</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="27">
         <v>65654.267000000007</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="27">
         <v>-19308.857</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="27">
         <v>22559.368999999999</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="27">
         <v>10225.522000000001</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="27">
         <v>-680.62099999999998</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="61">
         <v>6085.9920000000002</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="27">
         <v>-2621.7489999999998</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="27">
         <v>-16873.167000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="27">
         <v>49975.197</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="27">
         <v>61791.303999999996</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="27">
         <v>66664.826000000001</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="27">
         <v>-21149.587</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="27">
         <v>24068.832999999999</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="27">
         <v>8621.2270000000008</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="27">
         <v>-2118.2759999999998</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="61">
         <v>6309.34</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="27">
         <v>-2768.8829999999998</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="27">
         <v>-11877.525</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="27">
         <v>58287.067999999999</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="27">
         <v>75278.202999999994</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="27">
         <v>78361.774000000005</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="27">
         <v>-21365.151999999998</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="27">
         <v>27518.445</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="27">
         <v>8908.17</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="27">
         <v>-2476.8150000000001</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="61">
         <v>8376.8989999999994</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="27">
         <v>-2537.2489999999998</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="27">
         <v>-15834.057000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="10" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="27">
         <v>49215.665000000001</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="27">
         <v>72688.744000000006</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="27">
         <v>82699.740000000005</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="27">
         <v>-21350.343000000001</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="27">
         <v>23577.079000000002</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="27">
         <v>8907.7119999999995</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="27">
         <v>-3785.9409999999998</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="61">
         <v>6385.48</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="27">
         <v>-3302.78</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="27">
         <v>-21655.126</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="27">
         <v>43505.87</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="27">
         <v>63143.357000000004</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="27">
         <v>73657.986999999994</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="27">
         <v>-20773.154999999999</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="27">
         <v>18969.386999999999</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="27">
         <v>10261.616</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="27">
         <v>-823.61599999999999</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="61">
         <v>11397.311</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="27">
         <v>-6760.1779999999999</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="27">
         <v>-18777.554</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="27">
         <v>58978.300999999999</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="27">
         <v>66273.407999999996</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="27">
         <v>86572.869000000006</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="27">
         <v>-22502.510999999999</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="27">
         <v>17314.191999999999</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="27">
         <v>10094.838</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="27">
         <v>-5469.87</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="61">
         <v>18036.373</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="27">
         <v>-8653.7669999999998</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="27">
         <v>-11093.361999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="27">
         <v>64413.652000000002</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="27">
         <v>77767.226999999999</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="27">
         <v>104680.758</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="27">
         <v>-26910.328000000001</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="27">
         <v>23008.91</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="27">
         <v>13645.421</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="27">
         <v>-10499.38</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="61">
         <v>26427.202000000001</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="27">
         <v>-8846.77</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="27">
         <v>-19706.953000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="27">
         <v>51332.707999999999</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="27">
         <v>78722.092000000004</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="27">
         <v>100367.216</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="27">
         <v>-21017.13</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="27">
         <v>26671.973999999998</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="27">
         <v>16997.14</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="27">
         <v>-12083.304</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="61">
         <v>29361.077000000001</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="27">
         <v>-9972.643</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="27">
         <v>-29253.248</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="27">
         <v>80788.322</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="27">
         <v>81067.997000000003</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="27">
         <v>80520.837</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="27">
         <v>-12909.548000000001</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="27">
         <v>35243.453000000001</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="27">
         <v>20214.030999999999</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="27">
         <v>-10211.473</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="61">
         <v>35352.309000000001</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="27">
         <v>-4322.6610000000001</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="27">
         <v>-20595.583999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:21" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="29">
+      <c r="B16" s="27">
         <v>80630.414000000004</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="27">
         <v>47874.949000000001</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="27">
         <v>69985.025999999998</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="27">
         <v>-20616.745999999999</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="27">
         <v>38499.182000000001</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="27">
         <v>24038.538</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H16" s="27">
         <v>-22914.278999999999</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="61">
         <v>64906.366999999998</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="27">
         <v>-7366.8239999999996</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="27">
         <v>-18830.085999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:11" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="28">
         <v>11500.768</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="28">
         <v>5255.0739999999996</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="28">
         <v>6676.0460000000003</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="28">
         <v>-1601.9929999999999</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="28">
         <v>3209.556</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="28">
         <v>1896.867</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="28">
         <v>-1729.816</v>
       </c>
-      <c r="I17" s="30">
+      <c r="I17" s="62">
         <v>8610.6640000000007</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J17" s="28">
         <v>-246.40199999999999</v>
       </c>
-      <c r="K17" s="30">
+      <c r="K17" s="28">
         <v>-2030.4369999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="28">
         <v>7125.9709999999995</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="28">
         <v>4268.7110000000002</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="28">
         <v>7039.2740000000003</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="28">
         <v>-1757.0340000000001</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="28">
         <v>2969.1489999999999</v>
       </c>
-      <c r="G18" s="30">
+      <c r="G18" s="28">
         <v>2028.93</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="28">
         <v>-2199.3310000000001</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="62">
         <v>5403.5780000000004</v>
       </c>
-      <c r="J18" s="30">
+      <c r="J18" s="28">
         <v>-482.69099999999997</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="28">
         <v>-1539.212</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="21" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="28">
         <v>7040.3450000000003</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="28">
         <v>3457.94</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="28">
         <v>6736.4719999999998</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="28">
         <v>-2046.501</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>3410.2420000000002</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="28">
         <v>1956.566</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="28">
         <v>-3194.8020000000001</v>
       </c>
-      <c r="I19" s="30">
+      <c r="I19" s="62">
         <v>5423.317</v>
       </c>
-      <c r="J19" s="30">
+      <c r="J19" s="28">
         <v>-921.29600000000005</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="28">
         <v>-1274.203</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="28">
         <v>7940.59</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <v>5082.9160000000002</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>6610.4620000000004</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="28">
         <v>-1476.509</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="28">
         <v>3566.0079999999998</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="28">
         <v>2040.171</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="28">
         <v>-2067.9760000000001</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="62">
         <v>5594.1869999999999</v>
       </c>
-      <c r="J20" s="30">
+      <c r="J20" s="28">
         <v>-886.19899999999996</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="28">
         <v>-1323.6469999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="28">
         <v>6059.9080000000004</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="28">
         <v>3495.549</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="28">
         <v>6382.6540000000005</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="28">
         <v>-2462.2249999999999</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="28">
         <v>4542.7809999999999</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="28">
         <v>2851.2710000000002</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="28">
         <v>-2732.5610000000001</v>
       </c>
-      <c r="I21" s="30">
+      <c r="I21" s="62">
         <v>6203.6480000000001</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J21" s="28">
         <v>-1472.133</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="28">
         <v>-1532.0550000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="22" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="36" t="s">
+    <row r="22" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A22" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="27">
         <v>86890.429000000004</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C22" s="27">
         <v>18356.857</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="27">
         <v>49096.595000000001</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="27">
         <v>-16359.15</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="27">
         <v>37693.311999999998</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="27">
         <v>17244.258999999998</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="27">
         <v>-23566.048999999999</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="61">
         <v>85365.92</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="27">
         <v>-8496.0550000000003</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K22" s="27">
         <v>-13458.55</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="28">
         <v>10064.271000000001</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="28">
         <v>3931.7460000000001</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="28">
         <v>4557.884</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="28">
         <v>-812.94200000000001</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="28">
         <v>4817.6559999999999</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="28">
         <v>2477.8220000000001</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="28">
         <v>-2367.0520000000001</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="62">
         <v>5635.7120000000004</v>
       </c>
-      <c r="J23" s="30">
+      <c r="J23" s="28">
         <v>-135.845</v>
       </c>
-      <c r="K23" s="30">
+      <c r="K23" s="28">
         <v>-1215.3499999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="28">
         <v>6631.4390000000003</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="28">
         <v>1529.546</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="28">
         <v>5810.34</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="28">
         <v>-2488.2550000000001</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="28">
         <v>3260.3290000000002</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="28">
         <v>1936.376</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="28">
         <v>-2312.8809999999999</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="62">
         <v>8077.41</v>
       </c>
-      <c r="J24" s="30">
+      <c r="J24" s="28">
         <v>-1356.155</v>
       </c>
-      <c r="K24" s="30">
+      <c r="K24" s="28">
         <v>-2061.549</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="28">
         <v>6930.4089999999997</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="28">
         <v>2549.4839999999999</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="28">
         <v>6485.9080000000004</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="28">
         <v>-2707.404</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="28">
         <v>5007.8410000000003</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="28">
         <v>2254.3820000000001</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="28">
         <v>-2835.7260000000001</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="62">
         <v>8368.2759999999998</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="28">
         <v>-1318.134</v>
       </c>
-      <c r="K25" s="30">
+      <c r="K25" s="28">
         <v>-1833.1179999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A26" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="67">
+        <v>7397.0829999999996</v>
+      </c>
+      <c r="C26" s="67">
+        <v>1012.479</v>
+      </c>
+      <c r="D26" s="67">
+        <v>6213.7849999999999</v>
+      </c>
+      <c r="E26" s="67">
+        <v>-2414.8870000000002</v>
+      </c>
+      <c r="F26" s="67">
+        <v>5354.2209999999995</v>
+      </c>
+      <c r="G26" s="67">
+        <v>1932.364</v>
+      </c>
+      <c r="H26" s="67">
+        <v>-2316.6680000000001</v>
+      </c>
+      <c r="I26" s="67">
+        <v>9067.2739999999994</v>
+      </c>
+      <c r="J26" s="67">
+        <v>-1430.4739999999999</v>
+      </c>
+      <c r="K26" s="67">
+        <v>-1806.8030000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="30">
-        <v>7397.0829999999996</v>
-      </c>
-      <c r="C26" s="30">
-        <v>1012.479</v>
-      </c>
-      <c r="D26" s="30">
-        <v>6213.7849999999999</v>
-      </c>
-      <c r="E26" s="30">
-        <v>-2414.8870000000002</v>
-      </c>
-      <c r="F26" s="30">
-        <v>5354.2209999999995</v>
-      </c>
-      <c r="G26" s="30">
-        <v>1932.364</v>
-      </c>
-      <c r="H26" s="30">
-        <v>-2316.6680000000001</v>
-      </c>
-      <c r="I26" s="30">
-        <v>9067.2739999999994</v>
-      </c>
-      <c r="J26" s="30">
-        <v>-1430.4739999999999</v>
-      </c>
-      <c r="K26" s="30">
-        <v>-1806.8030000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="22" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="28">
+        <v>12619.18</v>
+      </c>
+      <c r="C27" s="28">
+        <v>2966.4969999999998</v>
+      </c>
+      <c r="D27" s="28">
+        <v>6565.3140000000003</v>
+      </c>
+      <c r="E27" s="28">
+        <v>-1796.09</v>
+      </c>
+      <c r="F27" s="28">
+        <v>4929.9110000000001</v>
+      </c>
+      <c r="G27" s="28">
+        <v>1681.028</v>
+      </c>
+      <c r="H27" s="28">
+        <v>-3054.895</v>
+      </c>
+      <c r="I27" s="62">
+        <v>10707.200999999999</v>
+      </c>
+      <c r="J27" s="28">
+        <v>-562.09400000000005</v>
+      </c>
+      <c r="K27" s="28">
+        <v>-1410.1130000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="30">
-        <v>12619.18</v>
-      </c>
-      <c r="C27" s="30">
-        <v>2966.4969999999998</v>
-      </c>
-      <c r="D27" s="30">
-        <v>6565.3140000000003</v>
-      </c>
-      <c r="E27" s="30">
-        <v>-1796.09</v>
-      </c>
-      <c r="F27" s="30">
-        <v>4929.9110000000001</v>
-      </c>
-      <c r="G27" s="30">
-        <v>1681.028</v>
-      </c>
-      <c r="H27" s="30">
-        <v>-3054.895</v>
-      </c>
-      <c r="I27" s="30">
-        <v>10707.200999999999</v>
-      </c>
-      <c r="J27" s="30">
-        <v>-562.09400000000005</v>
-      </c>
-      <c r="K27" s="30">
-        <v>-1410.1130000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="28">
+        <v>12077.311</v>
+      </c>
+      <c r="C28" s="28">
+        <v>1750.518</v>
+      </c>
+      <c r="D28" s="28">
+        <v>6330.4880000000003</v>
+      </c>
+      <c r="E28" s="28">
+        <v>-2020.4649999999999</v>
+      </c>
+      <c r="F28" s="28">
+        <v>3959.4960000000001</v>
+      </c>
+      <c r="G28" s="28">
+        <v>2406.297</v>
+      </c>
+      <c r="H28" s="28">
+        <v>-3377.6640000000002</v>
+      </c>
+      <c r="I28" s="62">
+        <v>13375.596</v>
+      </c>
+      <c r="J28" s="28">
+        <v>-1916.644</v>
+      </c>
+      <c r="K28" s="28">
+        <v>-1890.6880000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="30">
-        <v>12077.311</v>
-      </c>
-      <c r="C28" s="30">
-        <v>1750.518</v>
-      </c>
-      <c r="D28" s="30">
-        <v>6330.4880000000003</v>
-      </c>
-      <c r="E28" s="30">
-        <v>-2020.4649999999999</v>
-      </c>
-      <c r="F28" s="30">
-        <v>3959.4960000000001</v>
-      </c>
-      <c r="G28" s="30">
-        <v>2406.297</v>
-      </c>
-      <c r="H28" s="30">
-        <v>-3377.6640000000002</v>
-      </c>
-      <c r="I28" s="30">
-        <v>13375.596</v>
-      </c>
-      <c r="J28" s="30">
-        <v>-1916.644</v>
-      </c>
-      <c r="K28" s="30">
-        <v>-1890.6880000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="28">
+        <v>14342.050999999999</v>
+      </c>
+      <c r="C29" s="28">
+        <v>1643.046</v>
+      </c>
+      <c r="D29" s="28">
+        <v>5857.0190000000002</v>
+      </c>
+      <c r="E29" s="28">
+        <v>-2322.7809999999999</v>
+      </c>
+      <c r="F29" s="28">
+        <v>5739.5290000000005</v>
+      </c>
+      <c r="G29" s="28">
+        <v>2648.683</v>
+      </c>
+      <c r="H29" s="28">
+        <v>-3643.8620000000001</v>
+      </c>
+      <c r="I29" s="62">
+        <v>14473.178</v>
+      </c>
+      <c r="J29" s="28">
+        <v>-756.55899999999997</v>
+      </c>
+      <c r="K29" s="28">
+        <v>-1669.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="30">
-        <v>14342.050999999999</v>
-      </c>
-      <c r="C29" s="30">
-        <v>1643.046</v>
-      </c>
-      <c r="D29" s="30">
-        <v>5857.0190000000002</v>
-      </c>
-      <c r="E29" s="30">
-        <v>-2322.7809999999999</v>
-      </c>
-      <c r="F29" s="30">
-        <v>5739.5290000000005</v>
-      </c>
-      <c r="G29" s="30">
-        <v>2648.683</v>
-      </c>
-      <c r="H29" s="30">
-        <v>-3643.8620000000001</v>
-      </c>
-      <c r="I29" s="30">
-        <v>14473.178</v>
-      </c>
-      <c r="J29" s="30">
-        <v>-756.55899999999997</v>
-      </c>
-      <c r="K29" s="30">
-        <v>-1669.56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="28">
+        <v>16828.685000000001</v>
+      </c>
+      <c r="C30" s="28">
+        <v>2973.5410000000002</v>
+      </c>
+      <c r="D30" s="28">
+        <v>7275.857</v>
+      </c>
+      <c r="E30" s="28">
+        <v>-1796.326</v>
+      </c>
+      <c r="F30" s="28">
+        <v>4624.3289999999997</v>
+      </c>
+      <c r="G30" s="28">
+        <v>1907.307</v>
+      </c>
+      <c r="H30" s="28">
+        <v>-3657.3009999999999</v>
+      </c>
+      <c r="I30" s="62">
+        <v>15661.272999999999</v>
+      </c>
+      <c r="J30" s="28">
+        <v>-1020.15</v>
+      </c>
+      <c r="K30" s="28">
+        <v>-1571.3689999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="19" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A31" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="30">
-        <v>16828.685000000001</v>
-      </c>
-      <c r="C30" s="30">
-        <v>2973.5410000000002</v>
-      </c>
-      <c r="D30" s="30">
-        <v>7275.857</v>
-      </c>
-      <c r="E30" s="30">
-        <v>-1796.326</v>
-      </c>
-      <c r="F30" s="30">
-        <v>4624.3289999999997</v>
-      </c>
-      <c r="G30" s="30">
-        <v>1907.307</v>
-      </c>
-      <c r="H30" s="30">
-        <v>-3657.3009999999999</v>
-      </c>
-      <c r="I30" s="30">
-        <v>15661.272999999999</v>
-      </c>
-      <c r="J30" s="30">
-        <v>-1020.15</v>
-      </c>
-      <c r="K30" s="30">
-        <v>-1571.3689999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="20" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A31" s="37" t="s">
+      <c r="B31" s="29">
+        <v>2486.634</v>
+      </c>
+      <c r="C31" s="30">
+        <v>1330.4949999999999</v>
+      </c>
+      <c r="D31" s="30">
+        <v>1418.838</v>
+      </c>
+      <c r="E31" s="30">
+        <v>526.45500000000004</v>
+      </c>
+      <c r="F31" s="30">
+        <v>-1115.2</v>
+      </c>
+      <c r="G31" s="30">
+        <v>-741.37599999999998</v>
+      </c>
+      <c r="H31" s="30">
+        <v>-13.439</v>
+      </c>
+      <c r="I31" s="63">
+        <v>1188.095</v>
+      </c>
+      <c r="J31" s="30">
+        <v>-263.59100000000001</v>
+      </c>
+      <c r="K31" s="30">
+        <v>98.191000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="19" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A32" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="31">
-        <v>2486.634</v>
-      </c>
-      <c r="C31" s="32">
-        <v>1330.4949999999999</v>
-      </c>
-      <c r="D31" s="32">
-        <v>1418.838</v>
-      </c>
-      <c r="E31" s="32">
-        <v>526.45500000000004</v>
-      </c>
-      <c r="F31" s="32">
-        <v>-1115.2</v>
-      </c>
-      <c r="G31" s="32">
-        <v>-741.37599999999998</v>
-      </c>
-      <c r="H31" s="32">
-        <v>-13.439</v>
-      </c>
-      <c r="I31" s="32">
-        <v>1188.095</v>
-      </c>
-      <c r="J31" s="32">
-        <v>-263.59100000000001</v>
-      </c>
-      <c r="K31" s="32">
-        <v>98.191000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="21" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A32" s="38" t="s">
+      <c r="B32" s="31">
+        <v>5327.9170000000004</v>
+      </c>
+      <c r="C32" s="32">
+        <v>-2281.5329999999999</v>
+      </c>
+      <c r="D32" s="32">
+        <v>599.81100000000004</v>
+      </c>
+      <c r="E32" s="32">
+        <v>-194.333</v>
+      </c>
+      <c r="F32" s="32">
+        <v>1414.7729999999999</v>
+      </c>
+      <c r="G32" s="32">
+        <v>10.44</v>
+      </c>
+      <c r="H32" s="32">
+        <v>-1927.4849999999999</v>
+      </c>
+      <c r="I32" s="64">
+        <v>7050.6090000000004</v>
+      </c>
+      <c r="J32" s="32">
+        <v>-773.74800000000005</v>
+      </c>
+      <c r="K32" s="32">
+        <v>459.06799999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" s="19" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A33" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="33">
-        <v>5327.9170000000004</v>
-      </c>
-      <c r="C32" s="34">
-        <v>-2281.5329999999999</v>
-      </c>
-      <c r="D32" s="34">
-        <v>599.81100000000004</v>
-      </c>
-      <c r="E32" s="34">
-        <v>-194.333</v>
-      </c>
-      <c r="F32" s="34">
-        <v>1414.7729999999999</v>
-      </c>
-      <c r="G32" s="34">
-        <v>10.44</v>
-      </c>
-      <c r="H32" s="34">
-        <v>-1927.4849999999999</v>
-      </c>
-      <c r="I32" s="34">
-        <v>7050.6090000000004</v>
-      </c>
-      <c r="J32" s="34">
-        <v>-773.74800000000005</v>
-      </c>
-      <c r="K32" s="34">
-        <v>459.06799999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" s="21" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A33" s="39" t="s">
+      <c r="B33" s="33">
+        <v>34426.828999999998</v>
+      </c>
+      <c r="C33" s="33">
+        <v>-13212.976000000001</v>
+      </c>
+      <c r="D33" s="33">
+        <v>5880.4309999999996</v>
+      </c>
+      <c r="E33" s="33">
+        <v>-3484.6729999999998</v>
+      </c>
+      <c r="F33" s="33">
+        <v>13682.31</v>
+      </c>
+      <c r="G33" s="33">
+        <v>2082.6590000000001</v>
+      </c>
+      <c r="H33" s="33">
+        <v>-10846.44</v>
+      </c>
+      <c r="I33" s="65">
+        <v>43084.283000000003</v>
+      </c>
+      <c r="J33" s="33">
+        <v>-4891.55</v>
+      </c>
+      <c r="K33" s="33">
+        <v>-297.58100000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" s="19" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="35">
-        <v>34426.828999999998</v>
-      </c>
-      <c r="C33" s="35">
-        <v>-13212.976000000001</v>
-      </c>
-      <c r="D33" s="35">
-        <v>5880.4309999999996</v>
-      </c>
-      <c r="E33" s="35">
-        <v>-3484.6729999999998</v>
-      </c>
-      <c r="F33" s="35">
-        <v>13682.31</v>
-      </c>
-      <c r="G33" s="35">
-        <v>2082.6590000000001</v>
-      </c>
-      <c r="H33" s="35">
-        <v>-10846.44</v>
-      </c>
-      <c r="I33" s="35">
-        <v>43084.283000000003</v>
-      </c>
-      <c r="J33" s="35">
-        <v>-4891.55</v>
-      </c>
-      <c r="K33" s="35">
-        <v>-297.58100000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" s="20" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-    </row>
-    <row r="35" spans="1:24" s="25" customFormat="1" ht="14.1" customHeight="1">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
-    </row>
-    <row r="36" spans="1:24" s="25" customFormat="1">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
-    </row>
-    <row r="37" spans="1:24" s="25" customFormat="1">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-    </row>
-    <row r="38" spans="1:24" s="25" customFormat="1">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-    </row>
-    <row r="39" spans="1:24" s="25" customFormat="1">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
-    </row>
-    <row r="40" spans="1:24" s="25" customFormat="1">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="20"/>
-      <c r="X40" s="20"/>
-    </row>
-    <row r="41" spans="1:24" s="25" customFormat="1">
-      <c r="A41" s="23"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="20"/>
-      <c r="S41" s="20"/>
-      <c r="T41" s="20"/>
-      <c r="U41" s="20"/>
-      <c r="V41" s="20"/>
-      <c r="W41" s="20"/>
-      <c r="X41" s="20"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:24" s="23" customFormat="1" ht="14.1" customHeight="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+    </row>
+    <row r="36" spans="1:24" s="23" customFormat="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+    </row>
+    <row r="37" spans="1:24" s="23" customFormat="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+    </row>
+    <row r="38" spans="1:24" s="23" customFormat="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+    </row>
+    <row r="39" spans="1:24" s="23" customFormat="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+    </row>
+    <row r="40" spans="1:24" s="23" customFormat="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+    </row>
+    <row r="41" spans="1:24" s="23" customFormat="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
     </row>
     <row r="42" spans="1:24">
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="7"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="8"/>
-      <c r="X43" s="8"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="7"/>
+      <c r="X43" s="7"/>
     </row>
     <row r="44" spans="1:24">
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="8"/>
-      <c r="W44" s="8"/>
-      <c r="X44" s="8"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
     </row>
     <row r="45" spans="1:24">
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="8"/>
-      <c r="W45" s="8"/>
-      <c r="X45" s="8"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
     </row>
     <row r="46" spans="1:24">
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="8"/>
-      <c r="W46" s="8"/>
-      <c r="X46" s="8"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
-      <c r="X47" s="8"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
     </row>
     <row r="48" spans="1:24">
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
     </row>
     <row r="49" spans="2:24">
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="8"/>
-      <c r="X49" s="8"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="7"/>
     </row>
     <row r="50" spans="2:24">
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="8"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>